<commit_message>
removed nozzles as user inputs for ICAES, now user directly inputs the mass loading (ML) per stage
results verified with tests/test_ICAES.py
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207800B6-A37A-45D9-B94A-C189D749B13B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A856E2D0-391A-4644-B3AB-B7ECAD4E8311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,19 +16,11 @@
     <sheet name="sensitivity_variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="52">
   <si>
     <t>debug</t>
   </si>
@@ -135,39 +127,9 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>nozzles_cmp1</t>
-  </si>
-  <si>
-    <t>nozzles_exp1</t>
-  </si>
-  <si>
-    <t>nozzles_cmp5</t>
-  </si>
-  <si>
-    <t>nozzles_cmp4</t>
-  </si>
-  <si>
-    <t>nozzles_cmp3</t>
-  </si>
-  <si>
-    <t>nozzles_cmp2</t>
-  </si>
-  <si>
     <t>Unused</t>
   </si>
   <si>
-    <t>nozzles_exp2</t>
-  </si>
-  <si>
-    <t>nozzles_exp3</t>
-  </si>
-  <si>
-    <t>nozzles_exp4</t>
-  </si>
-  <si>
-    <t>nozzles_exp5</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -178,6 +140,42 @@
   </si>
   <si>
     <t>loss_gen</t>
+  </si>
+  <si>
+    <t>loss_m_air</t>
+  </si>
+  <si>
+    <t>mach_limit</t>
+  </si>
+  <si>
+    <t>ML_cmp1</t>
+  </si>
+  <si>
+    <t>ML_cmp2</t>
+  </si>
+  <si>
+    <t>ML_cmp3</t>
+  </si>
+  <si>
+    <t>ML_cmp4</t>
+  </si>
+  <si>
+    <t>ML_cmp5</t>
+  </si>
+  <si>
+    <t>ML_exp1</t>
+  </si>
+  <si>
+    <t>ML_exp2</t>
+  </si>
+  <si>
+    <t>ML_exp3</t>
+  </si>
+  <si>
+    <t>ML_exp4</t>
+  </si>
+  <si>
+    <t>Ml_exp5</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1053,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>26</v>
@@ -1191,7 +1189,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>0.05</v>
@@ -1207,7 +1205,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7">
         <v>2.5000000000000001E-2</v>
@@ -1226,7 +1224,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="4">
-        <v>0.26500000000000001</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>28</v>
@@ -1420,12 +1418,12 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="6">
-        <v>100</v>
-      </c>
-      <c r="C25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -1435,10 +1433,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="6">
-        <v>0.75</v>
+        <v>50</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>28</v>
@@ -1449,30 +1447,28 @@
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B28" s="6">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+        <v>0.75</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -1481,26 +1477,28 @@
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="6">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="6"/>
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B30" s="6">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>28</v>
@@ -1511,72 +1509,72 @@
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="A31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="6">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1">
         <v>-1</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1">
+      <c r="D33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1">
         <v>-1</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="6">
-        <v>15</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="6">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="6"/>
+      <c r="D34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B35" s="6">
         <v>1</v>
@@ -1590,37 +1588,67 @@
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="1">
+      <c r="A36" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="1">
         <v>-1</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="D38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="1">
         <v>-1</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>41</v>
+      <c r="D39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added demo for heat transfer models
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF368B9-B56B-42BD-A649-F7490769C9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA6925-520E-4313-8D21-136415928841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,11 +705,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1068,7 +1070,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,36 +1222,36 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="10">
         <v>0.05</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+      <c r="C10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="11">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -1614,192 +1616,192 @@
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="8">
         <v>0.75</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="9"/>
+      <c r="D36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="10" t="s">
+      <c r="D37" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>1</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="9"/>
+      <c r="D38" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>1</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="9"/>
+      <c r="D39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>1</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="9"/>
+      <c r="D40" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="9">
         <v>-1</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" s="10" t="s">
+      <c r="D41" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="9">
         <v>-1</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="D42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="8">
         <v>1</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="9"/>
+      <c r="D43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="8">
         <v>1</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="9"/>
+      <c r="D44" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="8">
         <v>1</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="9"/>
+      <c r="D45" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="9">
         <v>-1</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="10" t="s">
+      <c r="D46" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="9">
         <v>-1</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="10" t="s">
+      <c r="D47" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated heat transfer models
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA6925-520E-4313-8D21-136415928841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E90231-42B0-4349-9000-938A19515A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="71">
   <si>
     <t>debug</t>
   </si>
@@ -200,6 +200,39 @@
   </si>
   <si>
     <t>T_ocean</t>
+  </si>
+  <si>
+    <t>t_insul</t>
+  </si>
+  <si>
+    <t>k_insul</t>
+  </si>
+  <si>
+    <t>h_ocean</t>
+  </si>
+  <si>
+    <t>delta_p_cmp12</t>
+  </si>
+  <si>
+    <t>delta_p_cmp23</t>
+  </si>
+  <si>
+    <t>delta_p_cmp34</t>
+  </si>
+  <si>
+    <t>delta_p_cmp45</t>
+  </si>
+  <si>
+    <t>delta_p_exp12</t>
+  </si>
+  <si>
+    <t>delta_p_exp23</t>
+  </si>
+  <si>
+    <t>delta_p_exp34</t>
+  </si>
+  <si>
+    <t>delta_p_exp45</t>
   </si>
 </sst>
 </file>
@@ -695,7 +728,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,6 +745,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1067,15 +1101,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
@@ -1117,19 +1149,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="8">
         <v>100</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="5"/>
+      <c r="C3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1192,34 +1224,34 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="10">
         <v>15.4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="11">
         <v>2.75</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5"/>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -1229,7 +1261,7 @@
         <v>0.05</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>33</v>
@@ -1245,7 +1277,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>33</v>
@@ -1496,239 +1528,235 @@
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="8">
         <v>0.01</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="5"/>
+      <c r="C28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="8">
         <v>3.4700000000000002E-2</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="5"/>
+      <c r="C29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="5">
-        <v>100</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="5"/>
+      <c r="A30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="5">
+        <v>10</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B32" s="8">
         <v>0.72</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="C32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B33" s="8">
         <v>56.7</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="5">
-        <v>2.9</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="C33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="5">
-        <v>25</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="A34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="8">
+        <v>0.46</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2.9</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="5">
+        <v>25</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="5">
+        <v>3000</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B38" s="5">
         <v>290</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="8">
-        <v>1</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="8"/>
+      <c r="C38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="8">
+        <v>1</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B42" s="8">
         <v>1</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="8">
-        <v>1</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="9">
-        <v>-1</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="9">
-        <v>-1</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="C42" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B43" s="8">
         <v>1</v>
@@ -1742,66 +1770,243 @@
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="8">
+        <v>1</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B47" s="8">
         <v>1</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
+      <c r="C47" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B48" s="8">
         <v>1</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+      <c r="C48" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B49" s="9">
         <v>-1</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="9" t="s">
+      <c r="C49" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B50" s="9">
         <v>-1</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="9" t="s">
+      <c r="C50" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="8">
+        <v>0</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="8">
+        <v>0</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="9">
+        <v>-1</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created icaes2.py - an alternative isothermal caes representation where the polytropic index is specified instead of a water mass loading
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F5D180-4C53-45D5-8A5F-AFD5006BE20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4296F3-8099-419D-BC2F-6BDC521FB3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="72">
   <si>
     <t>debug</t>
   </si>
@@ -88,9 +88,6 @@
     <t>m_dot</t>
   </si>
   <si>
-    <t>eta_pump</t>
-  </si>
-  <si>
     <t>PR_type</t>
   </si>
   <si>
@@ -148,36 +145,6 @@
     <t>mach_limit</t>
   </si>
   <si>
-    <t>ML_cmp1</t>
-  </si>
-  <si>
-    <t>ML_cmp2</t>
-  </si>
-  <si>
-    <t>ML_cmp3</t>
-  </si>
-  <si>
-    <t>ML_cmp4</t>
-  </si>
-  <si>
-    <t>ML_cmp5</t>
-  </si>
-  <si>
-    <t>ML_exp1</t>
-  </si>
-  <si>
-    <t>ML_exp2</t>
-  </si>
-  <si>
-    <t>ML_exp3</t>
-  </si>
-  <si>
-    <t>ML_exp4</t>
-  </si>
-  <si>
-    <t>Ml_exp5</t>
-  </si>
-  <si>
     <t>t_pipe</t>
   </si>
   <si>
@@ -239,6 +206,36 @@
   </si>
   <si>
     <t>Not used for ICAES</t>
+  </si>
+  <si>
+    <t>n_cmp1</t>
+  </si>
+  <si>
+    <t>n_cmp2</t>
+  </si>
+  <si>
+    <t>n_cmp3</t>
+  </si>
+  <si>
+    <t>n_cmp4</t>
+  </si>
+  <si>
+    <t>n_cmp5</t>
+  </si>
+  <si>
+    <t>n_exp1</t>
+  </si>
+  <si>
+    <t>n_exp2</t>
+  </si>
+  <si>
+    <t>n_exp3</t>
+  </si>
+  <si>
+    <t>n_exp4</t>
+  </si>
+  <si>
+    <t>n_exp5</t>
   </si>
 </sst>
 </file>
@@ -1119,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1136,19 +1133,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1159,13 +1156,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1176,10 +1173,10 @@
         <v>100</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -1191,10 +1188,10 @@
         <v>16.850000000000001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -1206,10 +1203,10 @@
         <v>0.101325</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -1221,10 +1218,10 @@
         <v>16.850000000000001</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -1236,10 +1233,10 @@
         <v>0.101325</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4"/>
     </row>
@@ -1251,13 +1248,13 @@
         <v>15.4</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1268,43 +1265,43 @@
         <v>2.75</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="13">
         <v>0.05</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="14">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="6"/>
@@ -1317,10 +1314,10 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -1332,10 +1329,10 @@
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -1347,10 +1344,10 @@
         <v>1402.35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4"/>
     </row>
@@ -1362,10 +1359,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -1377,10 +1374,10 @@
         <v>14.73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="4"/>
     </row>
@@ -1392,10 +1389,10 @@
         <v>0.5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="4"/>
     </row>
@@ -1407,10 +1404,10 @@
         <v>2.3E-2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -1422,10 +1419,10 @@
         <v>10.617470333209738</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -1437,10 +1434,10 @@
         <v>122.937438838696</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4"/>
     </row>
@@ -1452,10 +1449,10 @@
         <v>62.44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="4"/>
     </row>
@@ -1467,10 +1464,10 @@
         <v>0.22919999999999999</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="4"/>
     </row>
@@ -1482,13 +1479,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1499,25 +1496,25 @@
         <v>38.33</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="4"/>
     </row>
@@ -1529,512 +1526,506 @@
         <v>276.882846301641</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="12">
         <v>0.3</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B28" s="7">
         <v>0.01</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B29" s="7">
         <v>3.4700000000000002E-2</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B30" s="7">
         <v>0.02</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B31" s="7">
         <v>10</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B32" s="7">
         <v>0.72</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B33" s="7">
         <v>56.7</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B34" s="7">
         <v>0.46</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B35" s="7">
         <v>2.9</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B36" s="7">
         <v>25</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B37" s="7">
         <v>3000</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B38" s="7">
         <v>290</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="12">
-        <v>0.75</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="12"/>
+      <c r="B39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A40" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="12">
+        <v>2</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="12">
-        <v>2</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" s="12"/>
+      <c r="A41" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="12"/>
+      <c r="A42" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="12">
-        <v>1</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="12"/>
+      <c r="A43" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B44" s="8">
         <v>-1</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="8">
+      <c r="A45" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="12"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="8">
         <v>-1</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="12">
-        <v>1</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="12"/>
+      <c r="C46" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="12"/>
+      <c r="A47" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="12">
-        <v>2</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="12"/>
+      <c r="A48" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B49" s="8">
         <v>-1</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B50" s="8">
+        <v>0</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="8">
         <v>-1</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="12">
-        <v>0</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" s="6"/>
+      <c r="C51" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="6"/>
+      <c r="A52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="8" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B53" s="8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="8" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B54" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E55" s="6"/>
+      <c r="A55" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="12">
-        <v>0</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E56" s="6"/>
+      <c r="A56" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="8">
+        <v>-1</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B57" s="8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="8">
-        <v>1</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated mid_atlantic post_processing to handle new case based results
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7155CE33-46B1-4D61-91C5-7F933C7FE21E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7B81BD-E48A-4C5A-A124-97746052621C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1279,7 +1279,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="13">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>27</v>
@@ -1295,7 +1295,7 @@
         <v>38</v>
       </c>
       <c r="B11" s="14">
-        <v>2.5000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>27</v>
@@ -1738,7 +1738,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>32</v>
@@ -1821,7 +1821,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated plotting and analysis
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/sensitivity/user_inputs.xlsx
+++ b/projects/mid_atlantic/sensitivity/user_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benne\PycharmProjects\caes\projects\mid_atlantic\sensitivity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7B81BD-E48A-4C5A-A124-97746052621C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F20B2DD-0C54-4D91-B519-2B514C89F512}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sensitivity_variables" sheetId="1" r:id="rId1"/>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>